<commit_message>
Adjusted Consent profiles. Added an example for TreatmentInstruction.
</commit_message>
<xml_diff>
--- a/Mappings/TreatmentInstruction - STU3.xlsx
+++ b/Mappings/TreatmentInstruction - STU3.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="94">
   <si>
     <t xml:space="preserve"># </t>
   </si>
@@ -268,9 +268,6 @@
     <t>Consent.purpose</t>
   </si>
   <si>
-    <t>Consent.noteExtension</t>
-  </si>
-  <si>
     <t>Consent.Source.Reference(Consent)</t>
   </si>
   <si>
@@ -286,7 +283,22 @@
     <t>gForge  #13313</t>
   </si>
   <si>
-    <t>Concent.extension</t>
+    <t>Concent.action</t>
+  </si>
+  <si>
+    <t>Concent.except.code.extenstion(constraints)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If modeling is ok: FHIR path expresions / invariants need to be added. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   IF TreatmentPermitted = yes, but then Consent.except.code needs to be given</t>
+  </si>
+  <si>
+    <t>Consent.extension(explanation)</t>
+  </si>
+  <si>
+    <t>Maybe not correctly mapped</t>
   </si>
 </sst>
 </file>
@@ -572,7 +584,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
@@ -625,9 +637,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -642,9 +651,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -666,9 +672,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
@@ -688,6 +691,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -994,7 +1009,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1014,15 +1029,15 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
       <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1035,17 +1050,17 @@
     </row>
     <row r="2" spans="1:12" ht="15">
       <c r="A2" s="3"/>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="31" t="s">
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="29" t="s">
         <v>80</v>
       </c>
       <c r="K2" s="4"/>
@@ -1055,24 +1070,24 @@
         <v>1</v>
       </c>
       <c r="B3" s="6"/>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="24" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="24" t="s">
         <v>24</v>
       </c>
       <c r="H3" s="9"/>
-      <c r="I3" s="30" t="s">
+      <c r="I3" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="18" t="s">
+      <c r="J3" s="43" t="s">
         <v>82</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="14.25">
@@ -1080,43 +1095,45 @@
         <v>2</v>
       </c>
       <c r="B4" s="12"/>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="24" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
-      <c r="G4" s="26" t="s">
+      <c r="G4" s="24" t="s">
         <v>25</v>
       </c>
       <c r="H4" s="16"/>
       <c r="I4" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="K4" s="10"/>
+      <c r="J4" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="5" spans="1:12" ht="14.25">
       <c r="A5" s="11">
         <v>3</v>
       </c>
       <c r="B5" s="12"/>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="24" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
-      <c r="G5" s="26" t="s">
+      <c r="G5" s="24" t="s">
         <v>26</v>
       </c>
       <c r="H5" s="16"/>
       <c r="I5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="18" t="s">
+      <c r="J5" s="44" t="s">
         <v>89</v>
       </c>
       <c r="K5" s="10"/>
@@ -1126,21 +1143,21 @@
         <v>4</v>
       </c>
       <c r="B6" s="12"/>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="24" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
-      <c r="G6" s="26" t="s">
+      <c r="G6" s="24" t="s">
         <v>22</v>
       </c>
       <c r="H6" s="16"/>
       <c r="I6" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="18" t="s">
-        <v>85</v>
+      <c r="J6" s="44" t="s">
+        <v>84</v>
       </c>
       <c r="K6" s="10"/>
     </row>
@@ -1149,21 +1166,21 @@
         <v>5</v>
       </c>
       <c r="B7" s="12"/>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="24" t="s">
         <v>16</v>
       </c>
       <c r="D7" s="13"/>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="24" t="s">
         <v>23</v>
       </c>
       <c r="H7" s="16"/>
       <c r="I7" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="18" t="s">
-        <v>86</v>
+      <c r="J7" s="44" t="s">
+        <v>85</v>
       </c>
       <c r="K7" s="10"/>
     </row>
@@ -1172,24 +1189,24 @@
         <v>6</v>
       </c>
       <c r="B8" s="12"/>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="24" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="13"/>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
-      <c r="G8" s="26" t="s">
+      <c r="G8" s="24" t="s">
         <v>8</v>
       </c>
       <c r="H8" s="16"/>
       <c r="I8" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="18" t="s">
-        <v>83</v>
+      <c r="J8" s="44" t="s">
+        <v>92</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="14.25">
@@ -1197,126 +1214,132 @@
         <v>7</v>
       </c>
       <c r="B9" s="12"/>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="24" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="13"/>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
-      <c r="G9" s="26" t="s">
+      <c r="G9" s="24" t="s">
         <v>27</v>
       </c>
       <c r="H9" s="16"/>
       <c r="I9" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="K9" s="32"/>
+      <c r="J9" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="K9" s="30"/>
     </row>
     <row r="10" spans="1:12" ht="14.25">
       <c r="A10" s="11">
         <v>8</v>
       </c>
       <c r="B10" s="12"/>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="24" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
-      <c r="G10" s="26" t="s">
+      <c r="G10" s="24" t="s">
         <v>28</v>
       </c>
       <c r="H10" s="16"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="18" t="s">
+      <c r="I10" s="40"/>
+      <c r="J10" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="K10" s="19"/>
+      <c r="K10" s="18"/>
     </row>
     <row r="11" spans="1:12" ht="15">
       <c r="A11" s="11">
         <v>9</v>
       </c>
       <c r="B11" s="12"/>
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="24" t="s">
         <v>19</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
-      <c r="G11" s="26" t="s">
+      <c r="G11" s="24" t="s">
         <v>29</v>
       </c>
       <c r="H11" s="16"/>
-      <c r="I11" s="11" t="s">
+      <c r="I11" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="J11" s="18" t="s">
+      <c r="J11" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="K11" s="36"/>
+      <c r="K11" s="33"/>
     </row>
     <row r="12" spans="1:12" ht="14.25">
       <c r="A12" s="11">
         <v>10</v>
       </c>
       <c r="B12" s="12"/>
-      <c r="D12" s="26" t="s">
+      <c r="D12" s="24" t="s">
         <v>20</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
-      <c r="G12" s="26" t="s">
+      <c r="G12" s="24" t="s">
         <v>30</v>
       </c>
       <c r="H12" s="16"/>
-      <c r="I12" s="11" t="s">
+      <c r="I12" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="J12" s="18" t="s">
+      <c r="J12" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="K12" s="19"/>
+      <c r="K12" s="18"/>
     </row>
     <row r="13" spans="1:12" ht="15">
-      <c r="A13" s="20">
+      <c r="A13" s="19">
         <v>11</v>
       </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="28" t="s">
+      <c r="B13" s="20"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="28" t="s">
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H13" s="23"/>
-      <c r="I13" s="20" t="s">
+      <c r="H13" s="22"/>
+      <c r="I13" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="J13" s="24" t="s">
+      <c r="J13" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="K13" s="35"/>
+      <c r="K13" s="42"/>
     </row>
     <row r="14" spans="1:12">
-      <c r="L14" s="25"/>
+      <c r="K14" t="s">
+        <v>90</v>
+      </c>
+      <c r="L14" s="23"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="B15" s="33"/>
+      <c r="B15" s="31"/>
+      <c r="K15" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="34"/>
+      <c r="A16" s="32"/>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="34"/>
+      <c r="A17" s="32"/>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="34"/>
+      <c r="A18" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1655,7 +1678,7 @@
       <c r="B7" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="29">
+      <c r="C7" s="27">
         <v>8601000000000000</v>
       </c>
       <c r="D7" t="s">

</xml_diff>

<commit_message>
Updated TreatmentInstruction. Three ZIB concepts are now made to extensions.
</commit_message>
<xml_diff>
--- a/Mappings/TreatmentInstruction - STU3.xlsx
+++ b/Mappings/TreatmentInstruction - STU3.xlsx
@@ -12,12 +12,12 @@
     <sheet name="BehandelingToegestaanCodelijst" sheetId="3" r:id="rId3"/>
     <sheet name="GeverifieerdBijCodelijst" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621" iterate="1"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="92">
   <si>
     <t xml:space="preserve"># </t>
   </si>
@@ -265,9 +265,6 @@
     <t>Consent.verificationExtension</t>
   </si>
   <si>
-    <t>Consent.purpose</t>
-  </si>
-  <si>
     <t>Consent.Source.Reference(Consent)</t>
   </si>
   <si>
@@ -277,18 +274,9 @@
     <t>Consent.period.end</t>
   </si>
   <si>
-    <t>gForge? Renaming purpose to context?</t>
-  </si>
-  <si>
     <t>gForge  #13313</t>
   </si>
   <si>
-    <t>Concent.action</t>
-  </si>
-  <si>
-    <t>Concent.except.code.extenstion(constraints)</t>
-  </si>
-  <si>
     <t xml:space="preserve">If modeling is ok: FHIR path expresions / invariants need to be added. </t>
   </si>
   <si>
@@ -298,7 +286,13 @@
     <t>Consent.extension(explanation)</t>
   </si>
   <si>
-    <t>Maybe not correctly mapped</t>
+    <t>Consent.extension</t>
+  </si>
+  <si>
+    <t>gForge #13540</t>
+  </si>
+  <si>
+    <t>Concent.except.extenstion</t>
   </si>
 </sst>
 </file>
@@ -1009,7 +1003,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1084,10 +1078,10 @@
         <v>5</v>
       </c>
       <c r="J3" s="37" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="14.25">
@@ -1109,10 +1103,10 @@
         <v>5</v>
       </c>
       <c r="J4" s="38" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="14.25">
@@ -1134,9 +1128,11 @@
         <v>9</v>
       </c>
       <c r="J5" s="38" t="s">
-        <v>89</v>
-      </c>
-      <c r="K5" s="10"/>
+        <v>91</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="6" spans="1:12" ht="14.25">
       <c r="A6" s="11">
@@ -1157,7 +1153,7 @@
         <v>6</v>
       </c>
       <c r="J6" s="38" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K6" s="10"/>
     </row>
@@ -1180,7 +1176,7 @@
         <v>6</v>
       </c>
       <c r="J7" s="38" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K7" s="10"/>
     </row>
@@ -1203,10 +1199,10 @@
         <v>9</v>
       </c>
       <c r="J8" s="38" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="14.25">
@@ -1228,7 +1224,7 @@
         <v>10</v>
       </c>
       <c r="J9" s="38" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K9" s="30"/>
     </row>
@@ -1322,14 +1318,14 @@
     </row>
     <row r="14" spans="1:12">
       <c r="K14" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="L14" s="23"/>
     </row>
     <row r="15" spans="1:12">
       <c r="B15" s="31"/>
       <c r="K15" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:12">

</xml_diff>